<commit_message>
Agrega update de perfil
</commit_message>
<xml_diff>
--- a/Archivos/TablaPesos.xlsx
+++ b/Archivos/TablaPesos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giannitapia/Desktop/IAPersonal/BasicStreamlit/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021FAE16-B361-4F4C-BBFF-875F36845B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98E87CD-35FA-5D4D-9C7E-65F58C16CC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -111,8 +111,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95EEE778-0FB1-469B-87B4-92A048EBDD5C}" name="Tabla1" displayName="Tabla1" ref="A1:C18" totalsRowShown="0">
-  <autoFilter ref="A1:C18" xr:uid="{95EEE778-0FB1-469B-87B4-92A048EBDD5C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95EEE778-0FB1-469B-87B4-92A048EBDD5C}" name="Tabla1" displayName="Tabla1" ref="A1:C29" totalsRowShown="0">
+  <autoFilter ref="A1:C29" xr:uid="{95EEE778-0FB1-469B-87B4-92A048EBDD5C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3DD57401-C29B-45D4-A53F-02325C3F4756}" name="Libras por Lado"/>
     <tableColumn id="2" xr3:uid="{3DCDB686-B24C-44D8-89FF-574625344035}" name="Libras Totales" dataDxfId="1">
@@ -441,20 +441,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -474,10 +474,11 @@
         <v>65</v>
       </c>
       <c r="C2" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29.483504050000001</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>15</v>
       </c>
@@ -486,10 +487,11 @@
         <v>75</v>
       </c>
       <c r="C3" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34.019427749999998</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20</v>
       </c>
@@ -498,10 +500,11 @@
         <v>85</v>
       </c>
       <c r="C4" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38.555351450000003</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>25</v>
       </c>
@@ -510,10 +513,11 @@
         <v>95</v>
       </c>
       <c r="C5" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43.091275150000001</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>30</v>
       </c>
@@ -522,10 +526,11 @@
         <v>105</v>
       </c>
       <c r="C6" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47.627198849999999</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>35</v>
       </c>
@@ -534,10 +539,11 @@
         <v>115</v>
       </c>
       <c r="C7" s="2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52.163122550000004</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>40</v>
       </c>
@@ -546,10 +552,11 @@
         <v>125</v>
       </c>
       <c r="C8" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>56.699046250000002</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>45</v>
       </c>
@@ -558,10 +565,11 @@
         <v>135</v>
       </c>
       <c r="C9" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>61.23496995</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>50</v>
       </c>
@@ -570,10 +578,11 @@
         <v>145</v>
       </c>
       <c r="C10" s="2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>65.770893650000005</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>55</v>
       </c>
@@ -582,10 +591,11 @@
         <v>155</v>
       </c>
       <c r="C11" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>70.306817350000003</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>60</v>
       </c>
@@ -594,10 +604,11 @@
         <v>165</v>
       </c>
       <c r="C12" s="2">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>74.842741050000001</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>65</v>
       </c>
@@ -606,10 +617,11 @@
         <v>175</v>
       </c>
       <c r="C13" s="2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79.378664749999999</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>70</v>
       </c>
@@ -618,10 +630,11 @@
         <v>185</v>
       </c>
       <c r="C14" s="2">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>83.914588450000011</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>75</v>
       </c>
@@ -630,10 +643,11 @@
         <v>195</v>
       </c>
       <c r="C15" s="2">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>88.450512150000009</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>80</v>
       </c>
@@ -642,10 +656,11 @@
         <v>205</v>
       </c>
       <c r="C16" s="2">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>92.986435850000007</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>85</v>
       </c>
@@ -654,10 +669,11 @@
         <v>215</v>
       </c>
       <c r="C17" s="2">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>97.522359550000004</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>90</v>
       </c>
@@ -666,11 +682,155 @@
         <v>225</v>
       </c>
       <c r="C18" s="2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
+        <v>102.05828325</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" ref="B19:B29" si="1">A19*2+45</f>
+        <v>235</v>
+      </c>
+      <c r="C19" s="2">
+        <v>106.59420695</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>245</v>
+      </c>
+      <c r="C20" s="2">
+        <v>111.13013065000001</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>105</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="C21" s="2">
+        <v>115.66605435000001</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>110</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="C22" s="2">
+        <v>120.20197805000001</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>115</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+      <c r="C23" s="2">
+        <v>124.73790175000001</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>120</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="1"/>
+        <v>285</v>
+      </c>
+      <c r="C24" s="2">
+        <v>129.27382545</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>125</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="1"/>
+        <v>295</v>
+      </c>
+      <c r="C25" s="2">
+        <v>133.80974915000002</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>130</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="1"/>
+        <v>305</v>
+      </c>
+      <c r="C26" s="2">
+        <v>138.34567285</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>135</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="1"/>
+        <v>315</v>
+      </c>
+      <c r="C27" s="2">
+        <v>142.88159655000001</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>140</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="1"/>
+        <v>325</v>
+      </c>
+      <c r="C28" s="2">
+        <v>147.41752025</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>145</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="1"/>
+        <v>335</v>
+      </c>
+      <c r="C29" s="2">
+        <v>151.95344395000001</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>